<commit_message>
adding more simulations, changed results and ruffing files
</commit_message>
<xml_diff>
--- a/results/Final_simulation_results_averaged.xlsx
+++ b/results/Final_simulation_results_averaged.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="25">
   <si>
     <t>Experiment type</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>best_boosted_380</t>
+  </si>
+  <si>
+    <t>best_boosted_100_mod_par</t>
   </si>
   <si>
     <t>WWW automatic</t>
@@ -172,14 +175,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF93C47D"/>
-        <bgColor rgb="FF93C47D"/>
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor theme="0"/>
+        <fgColor rgb="FF93C47D"/>
+        <bgColor rgb="FF93C47D"/>
       </patternFill>
     </fill>
     <fill>
@@ -312,23 +315,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="8" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
@@ -353,12 +362,6 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="5" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -592,13 +595,13 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.25"/>
+    <col customWidth="1" min="1" max="1" width="34.25"/>
     <col customWidth="1" min="2" max="2" width="25.75"/>
     <col customWidth="1" min="3" max="3" width="24.75"/>
     <col customWidth="1" min="4" max="4" width="16.88"/>
     <col customWidth="1" min="5" max="5" width="18.75"/>
     <col customWidth="1" min="6" max="6" width="16.5"/>
-    <col customWidth="1" min="7" max="7" width="25.0"/>
+    <col customWidth="1" min="7" max="7" width="28.0"/>
     <col customWidth="1" min="8" max="8" width="23.88"/>
     <col customWidth="1" min="11" max="11" width="17.0"/>
   </cols>
@@ -877,36 +880,56 @@
       <c r="L8" s="5"/>
     </row>
     <row r="9">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="17" t="s">
+      <c r="B9" s="15">
+        <v>0.009</v>
+      </c>
+      <c r="C9" s="16">
+        <v>783.6</v>
+      </c>
+      <c r="D9" s="16">
+        <v>973.6</v>
+      </c>
+      <c r="E9" s="16">
+        <v>83.8</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="9">
+        <v>0.0103</v>
+      </c>
+      <c r="I9" s="10">
+        <v>808.7</v>
+      </c>
+      <c r="J9" s="10">
+        <v>949.6</v>
+      </c>
+      <c r="K9" s="10">
+        <v>82.7</v>
+      </c>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="5"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="5"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="20" t="s">
+        <v>14</v>
+      </c>
       <c r="L10" s="5"/>
     </row>
     <row r="11">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -930,7 +953,7 @@
       <c r="E12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="18"/>
+      <c r="F12" s="19"/>
       <c r="G12" s="3" t="s">
         <v>0</v>
       </c>
@@ -943,7 +966,7 @@
       <c r="J12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K12" s="20" t="s">
+      <c r="K12" s="21" t="s">
         <v>4</v>
       </c>
       <c r="L12" s="5"/>
@@ -964,7 +987,7 @@
       <c r="E13" s="8">
         <v>141.3</v>
       </c>
-      <c r="F13" s="16"/>
+      <c r="F13" s="17"/>
       <c r="G13" s="6" t="s">
         <v>5</v>
       </c>
@@ -998,7 +1021,7 @@
       <c r="E14" s="12">
         <v>107.6</v>
       </c>
-      <c r="F14" s="16"/>
+      <c r="F14" s="17"/>
       <c r="G14" s="6" t="s">
         <v>6</v>
       </c>
@@ -1032,7 +1055,7 @@
       <c r="E15" s="12">
         <v>65.1</v>
       </c>
-      <c r="F15" s="16"/>
+      <c r="F15" s="17"/>
       <c r="G15" s="6" t="s">
         <v>7</v>
       </c>
@@ -1066,7 +1089,7 @@
       <c r="E16" s="11">
         <v>51.0</v>
       </c>
-      <c r="F16" s="16"/>
+      <c r="F16" s="17"/>
       <c r="G16" s="6" t="s">
         <v>8</v>
       </c>
@@ -1100,7 +1123,7 @@
       <c r="E17" s="12">
         <v>93.7</v>
       </c>
-      <c r="F17" s="16"/>
+      <c r="F17" s="17"/>
       <c r="G17" s="6" t="s">
         <v>9</v>
       </c>
@@ -1119,17 +1142,17 @@
       <c r="L17" s="5"/>
     </row>
     <row r="18">
-      <c r="A18" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="16"/>
-      <c r="G18" s="17" t="s">
+      <c r="A18" s="18" t="s">
         <v>15</v>
       </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="20" t="s">
+        <v>16</v>
+      </c>
       <c r="L18" s="5"/>
     </row>
     <row r="19">
-      <c r="A19" s="16"/>
+      <c r="A19" s="17"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -1152,31 +1175,21 @@
       <c r="L20" s="5"/>
     </row>
     <row r="21">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
+      <c r="F21" s="13"/>
       <c r="L21" s="5"/>
     </row>
     <row r="22">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
       <c r="L22" s="5"/>
     </row>
     <row r="23">
@@ -1209,11 +1222,11 @@
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="G9:K9"/>
     <mergeCell ref="A18:E18"/>
     <mergeCell ref="G18:K18"/>
     <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="G10:K10"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1234,204 +1247,204 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="21" t="s">
+      <c r="B1" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="22"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2">
-      <c r="A2" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="24">
+      <c r="A2" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="26">
         <v>2.15E-4</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2" s="27">
         <v>0.0139</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="26">
         <v>737.38</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="26">
         <v>827.63</v>
       </c>
-      <c r="F2" s="24">
+      <c r="F2" s="26">
         <v>275.98</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="24">
+      <c r="A3" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="26">
         <v>1.33E-4</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3" s="27">
         <v>0.0086</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="26">
         <v>655.83</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="26">
         <v>1070.33</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="26">
         <v>110.22</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="24">
+      <c r="A4" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="26">
         <v>-0.00319</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="27">
         <v>-0.1873</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="26">
         <v>520.19</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="26">
         <v>1007.41</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="26">
         <v>82.26</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="24">
+      <c r="A5" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="26">
         <v>1.01E-4</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="27">
         <v>0.0065</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="26">
         <v>351.49</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="26">
         <v>1416.73</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="26">
         <v>73.19</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="24">
+      <c r="A6" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="26">
         <v>1.83E-4</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="27">
         <v>0.0118</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="26">
         <v>379.76</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="26">
         <v>1323.01</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="26">
         <v>137.66</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="16"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="16"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="16"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="16"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="16"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="31" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="30"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="30"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="30"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="30"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="30"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
       <c r="E14" s="33"/>
-      <c r="F14" s="30"/>
+      <c r="F14" s="16"/>
     </row>
     <row r="15">
       <c r="A15" s="34" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B15" s="35"/>
       <c r="C15" s="35"/>

</xml_diff>